<commit_message>
WP3 variables added (Subtasks 3.1.1, 3.1.2, 3.1.3 and 3.1.4-diet)
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F65BF4-4F2A-8F41-B91B-C498B78D7D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="294">
   <si>
     <t>name</t>
   </si>
@@ -318,13 +312,598 @@
   </si>
   <si>
     <t>Unique identifier for id in Opal</t>
+  </si>
+  <si>
+    <t>no2_y</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>microg / m3</t>
+  </si>
+  <si>
+    <t>no2 value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>nox_y</t>
+  </si>
+  <si>
+    <t>nox value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10_y</t>
+  </si>
+  <si>
+    <t>pm10 value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25_y</t>
+  </si>
+  <si>
+    <t>pm25 value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pmcoarse_y</t>
+  </si>
+  <si>
+    <t>pmcoarse value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25abs_y</t>
+  </si>
+  <si>
+    <t>10-5m-1</t>
+  </si>
+  <si>
+    <t>pm25abs value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25cu_y</t>
+  </si>
+  <si>
+    <t>pm25cu value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25fe_y</t>
+  </si>
+  <si>
+    <t>pm25fe value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25k_y</t>
+  </si>
+  <si>
+    <t>pm25k value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25ni_y</t>
+  </si>
+  <si>
+    <t>pm25ni value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25s_y</t>
+  </si>
+  <si>
+    <t>pm25s value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25si_y</t>
+  </si>
+  <si>
+    <t>pm25si value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25v_y</t>
+  </si>
+  <si>
+    <t>pm25v value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25zn_y</t>
+  </si>
+  <si>
+    <t>pm25zn value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10cu_y</t>
+  </si>
+  <si>
+    <t>pm10cu value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10fe_y</t>
+  </si>
+  <si>
+    <t>pm10fe value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10k_y</t>
+  </si>
+  <si>
+    <t>pm10k value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10ni_y</t>
+  </si>
+  <si>
+    <t>pm10ni value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10s_y</t>
+  </si>
+  <si>
+    <t>pm10s value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10si_y</t>
+  </si>
+  <si>
+    <t>pm10si value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10v_y</t>
+  </si>
+  <si>
+    <t>pm10v value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10zn_y</t>
+  </si>
+  <si>
+    <t>pm10zn value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>popdens_y</t>
+  </si>
+  <si>
+    <t>people / km2</t>
+  </si>
+  <si>
+    <t>population density</t>
+  </si>
+  <si>
+    <t>bdens100_y</t>
+  </si>
+  <si>
+    <t>m2 / km2</t>
+  </si>
+  <si>
+    <t>building density within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>bdens300_y</t>
+  </si>
+  <si>
+    <t>building density within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>connind100_y</t>
+  </si>
+  <si>
+    <t>number / km2</t>
+  </si>
+  <si>
+    <t>connectivity density within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>connind300_y</t>
+  </si>
+  <si>
+    <t>connectivity density within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>bus_lines_100_y</t>
+  </si>
+  <si>
+    <t>length of public bus lines within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>bus_lines_300_y</t>
+  </si>
+  <si>
+    <t>length of public bus lines within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>bus_lines_500_y</t>
+  </si>
+  <si>
+    <t>length of public bus lines within a buffer of 500 m</t>
+  </si>
+  <si>
+    <t>bus_stops_100_y</t>
+  </si>
+  <si>
+    <t>number of public bus stops within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>bus_stops_300_y</t>
+  </si>
+  <si>
+    <t>number of public bus stops within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>bus_stops_500_y</t>
+  </si>
+  <si>
+    <t>number of public bus stops within a buffer of 500 m</t>
+  </si>
+  <si>
+    <t>fdensity300_y</t>
+  </si>
+  <si>
+    <t>number of facilities present within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>frichness300_y</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>number of different facility types present divided by the maximum potential number of facility types within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>landuseshan300_y</t>
+  </si>
+  <si>
+    <t>landuse Shannon's Evenness Index within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>walkability_mean_y</t>
+  </si>
+  <si>
+    <t>walkability index (as mean of deciles of facility richness index, landuse shannon's Evenness Index, population density, connectivity density) within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>agrgr_y</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>percentage of agrgr (agricultural areas, semi-natural areas and wetlands) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>airpt_y</t>
+  </si>
+  <si>
+    <t>percentage of airpt (airports) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>hdres_y</t>
+  </si>
+  <si>
+    <t>percentage of hdres (continuous urban fabric) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>indtr_y</t>
+  </si>
+  <si>
+    <t>percentage of indtr (industrial, commercial, public, military and private units) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>ldres_y</t>
+  </si>
+  <si>
+    <t>percentage of ldres (discontinuous dense/medium density/low density urban fabric) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>natgr_y</t>
+  </si>
+  <si>
+    <t>percentage of natgr (forests) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>other_y</t>
+  </si>
+  <si>
+    <t>percentage of other (mineral extraction and dump sites, construction sites, land without current use) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>port_y</t>
+  </si>
+  <si>
+    <t>percentage of port (port areas) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>trans_y</t>
+  </si>
+  <si>
+    <t>percentage of trans (road and rail network and associated land, fast transit roads and associated land, other roads and associated land, railways and associated land) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>urbgr_y</t>
+  </si>
+  <si>
+    <t>percentage of urbgr (green urban areas, sports and leisure facilities) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>vldres_y</t>
+  </si>
+  <si>
+    <t>percentage of vldres (discontinuous very low density urban fabric) land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>water_y</t>
+  </si>
+  <si>
+    <t>percentage of water land use within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>blue_dist_y</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> straight line distance to nearest blue space &gt; 5,000 m2</t>
+  </si>
+  <si>
+    <t>green_dist_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> straight line distance to nearest green space &gt; 5,000 m2</t>
+  </si>
+  <si>
+    <t>blue_size_y</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> area of closest blue space &gt; 5,000m2</t>
+  </si>
+  <si>
+    <t>green_size_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> area of closest green space &gt; 5,000m2</t>
+  </si>
+  <si>
+    <t>blueyn300_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is there a blue space  &gt; 5,000 m2 in a distance of 300 m?</t>
+  </si>
+  <si>
+    <t>greenyn300_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is there a green space  &gt; 5,000 m2 in a distance of 300 m?</t>
+  </si>
+  <si>
+    <t>ndvi100_y</t>
+  </si>
+  <si>
+    <t>ndvi value</t>
+  </si>
+  <si>
+    <t>average of NDVI values within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>ndvi300_y</t>
+  </si>
+  <si>
+    <t>average of NDVI values within a buffer of 300 m</t>
+  </si>
+  <si>
+    <t>ndvi500_y</t>
+  </si>
+  <si>
+    <t>average of NDVI values within a buffer of 500 m</t>
+  </si>
+  <si>
+    <t>lden_y</t>
+  </si>
+  <si>
+    <t>dB(A)</t>
+  </si>
+  <si>
+    <t>day-evening-night level</t>
+  </si>
+  <si>
+    <t>ln_y</t>
+  </si>
+  <si>
+    <t>night level</t>
+  </si>
+  <si>
+    <t>lden_c_y</t>
+  </si>
+  <si>
+    <t>categorized day-evening-night level</t>
+  </si>
+  <si>
+    <t>ln_c_y</t>
+  </si>
+  <si>
+    <t>categorized night level</t>
+  </si>
+  <si>
+    <t>noise_dist_y</t>
+  </si>
+  <si>
+    <t>straight distance to the nearest road with noise level</t>
+  </si>
+  <si>
+    <t>areases_tert_y</t>
+  </si>
+  <si>
+    <t>area-level SES indicator (deprivation index in tertiles)</t>
+  </si>
+  <si>
+    <t>areases_quint_y</t>
+  </si>
+  <si>
+    <t>area-level SES indicator (deprivation index in quintiles)</t>
+  </si>
+  <si>
+    <t>distinvnear6_y</t>
+  </si>
+  <si>
+    <t>m-1</t>
+  </si>
+  <si>
+    <t>inverse distance to nearest road</t>
+  </si>
+  <si>
+    <t>trafload100_y</t>
+  </si>
+  <si>
+    <t>veh / day m</t>
+  </si>
+  <si>
+    <t>total traffic load of all roads within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>trafmajorload100_y</t>
+  </si>
+  <si>
+    <t>total traffic load of major roads within a buffer of 100 m</t>
+  </si>
+  <si>
+    <t>trafnear_y</t>
+  </si>
+  <si>
+    <t>veh / day</t>
+  </si>
+  <si>
+    <t>traffic density on nearest road</t>
+  </si>
+  <si>
+    <t>foodenvdens300_y</t>
+  </si>
+  <si>
+    <t>number of facilities related to unhealthy food divided by the area of the 300 meters buffer</t>
+  </si>
+  <si>
+    <t>foodenvdensosm300_y</t>
+  </si>
+  <si>
+    <t>number of open street maps facilities related to unhealthy food divided by the area of the 300 meters buffer</t>
+  </si>
+  <si>
+    <t>tm_y</t>
+  </si>
+  <si>
+    <t>ºC</t>
+  </si>
+  <si>
+    <t>mean temperature</t>
+  </si>
+  <si>
+    <t>tmin_y</t>
+  </si>
+  <si>
+    <t>minimum temperature</t>
+  </si>
+  <si>
+    <t>tmax_y</t>
+  </si>
+  <si>
+    <t>maximum temperature</t>
+  </si>
+  <si>
+    <t>hum_y</t>
+  </si>
+  <si>
+    <t>mean relative humidity</t>
+  </si>
+  <si>
+    <t>hmin_y</t>
+  </si>
+  <si>
+    <t>minimum relative humidity</t>
+  </si>
+  <si>
+    <t>hmax_y</t>
+  </si>
+  <si>
+    <t>maximum relative humidity</t>
+  </si>
+  <si>
+    <t>uvddc_y</t>
+  </si>
+  <si>
+    <t>kJ / sq m</t>
+  </si>
+  <si>
+    <t>DNA-damage UV dose</t>
+  </si>
+  <si>
+    <t>uvdec_y</t>
+  </si>
+  <si>
+    <t>erythemal UV dose</t>
+  </si>
+  <si>
+    <t>uvdvc_y</t>
+  </si>
+  <si>
+    <t>vitamin-d UV dose</t>
+  </si>
+  <si>
+    <t>lst_y</t>
+  </si>
+  <si>
+    <t>land surface temperature</t>
+  </si>
+  <si>
+    <t>FALSO</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>&lt;50</t>
+  </si>
+  <si>
+    <t>50-54.9</t>
+  </si>
+  <si>
+    <t>55-59.9</t>
+  </si>
+  <si>
+    <t>60-64.9</t>
+  </si>
+  <si>
+    <t>65-69.9</t>
+  </si>
+  <si>
+    <t>&lt;55</t>
+  </si>
+  <si>
+    <t>70-74.9</t>
+  </si>
+  <si>
+    <t>&gt;75</t>
+  </si>
+  <si>
+    <t>low deprivated</t>
+  </si>
+  <si>
+    <t>medium deprivated</t>
+  </si>
+  <si>
+    <t>high deprivated</t>
+  </si>
+  <si>
+    <t>medium-low deprivated</t>
+  </si>
+  <si>
+    <t>medium-high deprivated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -388,7 +967,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -399,11 +978,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -796,7 +1378,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -840,7 +1422,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -861,23 +1443,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BG112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:D112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="15" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -946,7 +1528,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -961,7 +1543,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -976,7 +1558,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -991,7 +1573,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1006,7 +1588,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1021,7 +1603,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1036,7 +1618,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1051,7 +1633,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1066,7 +1648,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" ht="15" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1081,7 +1663,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1678,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -1111,7 +1693,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
@@ -1126,7 +1708,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1723,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1156,7 +1738,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" ht="15" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
@@ -1171,7 +1753,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>29</v>
       </c>
@@ -1186,7 +1768,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -1201,7 +1783,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1216,7 +1798,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1231,7 +1813,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1246,7 +1828,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
@@ -1261,7 +1843,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -1276,7 +1858,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -1291,7 +1873,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
@@ -1306,7 +1888,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>40</v>
       </c>
@@ -1321,7 +1903,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -1336,7 +1918,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
@@ -1351,7 +1933,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
@@ -1366,7 +1948,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1963,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
@@ -1395,6 +1977,1140 @@
         <v>51</v>
       </c>
       <c r="E31"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1">
+      <c r="A40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1">
+      <c r="A41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1">
+      <c r="A42" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1">
+      <c r="A43" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1">
+      <c r="A44" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1">
+      <c r="A45" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" customHeight="1">
+      <c r="A46" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1">
+      <c r="A47" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" customHeight="1">
+      <c r="A48" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" customHeight="1">
+      <c r="A49" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" customHeight="1">
+      <c r="A50" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" customHeight="1">
+      <c r="A51" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1">
+      <c r="A52" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" customHeight="1">
+      <c r="A53" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" customHeight="1">
+      <c r="A54" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1">
+      <c r="A55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1">
+      <c r="A56" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" customHeight="1">
+      <c r="A57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" customHeight="1">
+      <c r="A58" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1">
+      <c r="A59" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" customHeight="1">
+      <c r="A60" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" customHeight="1">
+      <c r="A61" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" customHeight="1">
+      <c r="A62" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" customHeight="1">
+      <c r="A63" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" customHeight="1">
+      <c r="A64" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" customHeight="1">
+      <c r="A65" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" customHeight="1">
+      <c r="A66" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" customHeight="1">
+      <c r="A67" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1">
+      <c r="A68" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" customHeight="1">
+      <c r="A69" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" customHeight="1">
+      <c r="A70" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" customHeight="1">
+      <c r="A71" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" customHeight="1">
+      <c r="A72" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" customHeight="1">
+      <c r="A73" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" customHeight="1">
+      <c r="A74" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" customHeight="1">
+      <c r="A75" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" customHeight="1">
+      <c r="A76" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" customHeight="1">
+      <c r="A77" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" customHeight="1">
+      <c r="A78" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15" customHeight="1">
+      <c r="A79" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" customHeight="1">
+      <c r="A80" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" customHeight="1">
+      <c r="A81" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" customHeight="1">
+      <c r="A82" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" customHeight="1">
+      <c r="A83" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" customHeight="1">
+      <c r="A84" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" customHeight="1">
+      <c r="A85" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" customHeight="1">
+      <c r="A86" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" customHeight="1">
+      <c r="A87" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" customHeight="1">
+      <c r="A88" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" customHeight="1">
+      <c r="A89" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" customHeight="1">
+      <c r="A90" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" customHeight="1">
+      <c r="A91" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" customHeight="1">
+      <c r="A92" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1">
+      <c r="A93" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1">
+      <c r="A94" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" customHeight="1">
+      <c r="A95" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1">
+      <c r="A96" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" customHeight="1">
+      <c r="A97" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" customHeight="1">
+      <c r="A98" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" customHeight="1">
+      <c r="A99" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" customHeight="1">
+      <c r="A100" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" customHeight="1">
+      <c r="A101" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" customHeight="1">
+      <c r="A102" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" customHeight="1">
+      <c r="A103" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" customHeight="1">
+      <c r="A104" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" customHeight="1">
+      <c r="A105" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" customHeight="1">
+      <c r="A106" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" customHeight="1">
+      <c r="A107" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" customHeight="1">
+      <c r="A108" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" customHeight="1">
+      <c r="A109" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" customHeight="1">
+      <c r="A110" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" customHeight="1">
+      <c r="A111" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" customHeight="1">
+      <c r="A112" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>277</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -1406,22 +3122,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A68" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:D107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="40.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="40.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1435,7 +3151,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +3165,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1463,7 +3179,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1477,7 +3193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1491,7 +3207,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1505,7 +3221,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1519,7 +3235,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1533,7 +3249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +3263,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1561,7 +3277,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1575,7 +3291,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1589,7 +3305,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1603,7 +3319,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1617,7 +3333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1631,7 +3347,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1645,7 +3361,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1659,7 +3375,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1673,7 +3389,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1687,7 +3403,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1701,7 +3417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1715,7 +3431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -1729,7 +3445,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -1743,7 +3459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1757,7 +3473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -1771,7 +3487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -1785,7 +3501,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
@@ -1799,7 +3515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1813,7 +3529,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>19</v>
       </c>
@@ -1827,7 +3543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>19</v>
       </c>
@@ -1841,7 +3557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>19</v>
       </c>
@@ -1855,7 +3571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +3585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
@@ -1883,7 +3599,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>20</v>
       </c>
@@ -1897,7 +3613,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>20</v>
       </c>
@@ -1911,7 +3627,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>20</v>
       </c>
@@ -1925,7 +3641,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>20</v>
       </c>
@@ -1939,7 +3655,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
@@ -1953,7 +3669,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>22</v>
       </c>
@@ -1967,7 +3683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>22</v>
       </c>
@@ -1981,7 +3697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>22</v>
       </c>
@@ -1995,7 +3711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>22</v>
       </c>
@@ -2009,7 +3725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
@@ -2023,7 +3739,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +3753,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>23</v>
       </c>
@@ -2051,7 +3767,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
@@ -2065,7 +3781,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -2079,7 +3795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="15" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
@@ -2093,7 +3809,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>
@@ -2107,7 +3823,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>23</v>
       </c>
@@ -2121,7 +3837,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>23</v>
       </c>
@@ -2135,7 +3851,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -2149,7 +3865,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="5" t="s">
         <v>25</v>
       </c>
@@ -2163,7 +3879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="5" t="s">
         <v>25</v>
       </c>
@@ -2177,7 +3893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
@@ -2191,7 +3907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="5" t="s">
         <v>25</v>
       </c>
@@ -2205,7 +3921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>26</v>
       </c>
@@ -2219,7 +3935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>26</v>
       </c>
@@ -2233,7 +3949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>26</v>
       </c>
@@ -2247,7 +3963,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
@@ -2261,7 +3977,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>26</v>
       </c>
@@ -2275,7 +3991,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>26</v>
       </c>
@@ -2289,7 +4005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>26</v>
       </c>
@@ -2303,7 +4019,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="2" t="s">
         <v>26</v>
       </c>
@@ -2317,7 +4033,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>26</v>
       </c>
@@ -2331,7 +4047,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>26</v>
       </c>
@@ -2345,7 +4061,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="5" t="s">
         <v>28</v>
       </c>
@@ -2359,7 +4075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="5" t="s">
         <v>28</v>
       </c>
@@ -2373,7 +4089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="5" t="s">
         <v>28</v>
       </c>
@@ -2387,7 +4103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="5" t="s">
         <v>28</v>
       </c>
@@ -2401,7 +4117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="15" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>29</v>
       </c>
@@ -2415,7 +4131,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>29</v>
       </c>
@@ -2429,7 +4145,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>29</v>
       </c>
@@ -2443,7 +4159,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="15" customHeight="1">
       <c r="A74" s="5" t="s">
         <v>31</v>
       </c>
@@ -2457,7 +4173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="5" t="s">
         <v>31</v>
       </c>
@@ -2471,7 +4187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="15" customHeight="1">
       <c r="A76" s="5" t="s">
         <v>31</v>
       </c>
@@ -2485,7 +4201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="15" customHeight="1">
       <c r="A77" s="5" t="s">
         <v>31</v>
       </c>
@@ -2499,7 +4215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="15" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>32</v>
       </c>
@@ -2513,7 +4229,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="15" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>32</v>
       </c>
@@ -2527,7 +4243,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="15" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>32</v>
       </c>
@@ -2541,7 +4257,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="5" t="s">
         <v>34</v>
       </c>
@@ -2555,7 +4271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="15" customHeight="1">
       <c r="A82" s="5" t="s">
         <v>34</v>
       </c>
@@ -2569,7 +4285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="15" customHeight="1">
       <c r="A83" s="5" t="s">
         <v>34</v>
       </c>
@@ -2583,7 +4299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="5" t="s">
         <v>34</v>
       </c>
@@ -2595,6 +4311,328 @@
       </c>
       <c r="D84" s="6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" customHeight="1">
+      <c r="A85" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" customHeight="1">
+      <c r="A86" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B86" s="3">
+        <v>0</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" customHeight="1">
+      <c r="A87" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" customHeight="1">
+      <c r="A88" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" customHeight="1">
+      <c r="A89" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" customHeight="1">
+      <c r="A90" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B90" s="3">
+        <v>2</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" customHeight="1">
+      <c r="A91" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B91" s="3">
+        <v>3</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" customHeight="1">
+      <c r="A92" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B92" s="3">
+        <v>4</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1">
+      <c r="A93" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B93" s="3">
+        <v>5</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1">
+      <c r="A94" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" customHeight="1">
+      <c r="A95" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B95" s="3">
+        <v>2</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1">
+      <c r="A96" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B96" s="3">
+        <v>3</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" customHeight="1">
+      <c r="A97" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B97" s="3">
+        <v>4</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" customHeight="1">
+      <c r="A98" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B98" s="3">
+        <v>5</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" customHeight="1">
+      <c r="A99" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B99" s="3">
+        <v>6</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" customHeight="1">
+      <c r="A100" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B100" s="3">
+        <v>1</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" customHeight="1">
+      <c r="A101" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B101" s="3">
+        <v>2</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" customHeight="1">
+      <c r="A102" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B102" s="3">
+        <v>3</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" customHeight="1">
+      <c r="A103" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B103" s="3">
+        <v>1</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" customHeight="1">
+      <c r="A104" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B104" s="3">
+        <v>2</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" customHeight="1">
+      <c r="A105" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B105" s="3">
+        <v>3</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" customHeight="1">
+      <c r="A106" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B106" s="3">
+        <v>4</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" customHeight="1">
+      <c r="A107" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B107" s="3">
+        <v>5</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WP3 variables checked: yearly-repeated variables rename, units for the variables of subtask 3.1.3  rewritten not using symbols
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="12315" activeTab="1"/>
+    <workbookView xWindow="12" yWindow="24" windowWidth="11724" windowHeight="9612" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="294">
   <si>
     <t>name</t>
   </si>
@@ -314,546 +314,207 @@
     <t>Unique identifier for id in Opal</t>
   </si>
   <si>
-    <t>no2_y</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
-    <t>microg / m3</t>
-  </si>
-  <si>
-    <t>no2 value (extrapolated back in time using ratio method)</t>
-  </si>
-  <si>
-    <t>nox_y</t>
-  </si>
-  <si>
-    <t>nox value (extrapolated back in time using ratio method)</t>
-  </si>
-  <si>
-    <t>pm10_y</t>
-  </si>
-  <si>
-    <t>pm10 value (extrapolated back in time using ratio method)</t>
-  </si>
-  <si>
-    <t>pm25_y</t>
-  </si>
-  <si>
-    <t>pm25 value (extrapolated back in time using ratio method)</t>
-  </si>
-  <si>
-    <t>pmcoarse_y</t>
-  </si>
-  <si>
-    <t>pmcoarse value (extrapolated back in time using ratio method)</t>
-  </si>
-  <si>
-    <t>pm25abs_y</t>
-  </si>
-  <si>
-    <t>10-5m-1</t>
-  </si>
-  <si>
-    <t>pm25abs value (extrapolated back in time using ratio method)</t>
-  </si>
-  <si>
-    <t>pm25cu_y</t>
-  </si>
-  <si>
     <t>pm25cu value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25fe_y</t>
-  </si>
-  <si>
     <t>pm25fe value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25k_y</t>
-  </si>
-  <si>
     <t>pm25k value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25ni_y</t>
-  </si>
-  <si>
     <t>pm25ni value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25s_y</t>
-  </si>
-  <si>
     <t>pm25s value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25si_y</t>
-  </si>
-  <si>
     <t>pm25si value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25v_y</t>
-  </si>
-  <si>
     <t>pm25v value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm25zn_y</t>
-  </si>
-  <si>
     <t>pm25zn value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10cu_y</t>
-  </si>
-  <si>
     <t>pm10cu value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10fe_y</t>
-  </si>
-  <si>
     <t>pm10fe value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10k_y</t>
-  </si>
-  <si>
     <t>pm10k value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10ni_y</t>
-  </si>
-  <si>
     <t>pm10ni value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10s_y</t>
-  </si>
-  <si>
     <t>pm10s value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10si_y</t>
-  </si>
-  <si>
     <t>pm10si value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10v_y</t>
-  </si>
-  <si>
     <t>pm10v value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>pm10zn_y</t>
-  </si>
-  <si>
     <t>pm10zn value (extrapolated back in time using ratio method)</t>
   </si>
   <si>
-    <t>popdens_y</t>
-  </si>
-  <si>
-    <t>people / km2</t>
-  </si>
-  <si>
     <t>population density</t>
   </si>
   <si>
-    <t>bdens100_y</t>
-  </si>
-  <si>
-    <t>m2 / km2</t>
-  </si>
-  <si>
     <t>building density within a buffer of 100 m</t>
   </si>
   <si>
-    <t>bdens300_y</t>
-  </si>
-  <si>
     <t>building density within a buffer of 300 m</t>
   </si>
   <si>
-    <t>connind100_y</t>
-  </si>
-  <si>
-    <t>number / km2</t>
-  </si>
-  <si>
     <t>connectivity density within a buffer of 100 m</t>
   </si>
   <si>
-    <t>connind300_y</t>
-  </si>
-  <si>
     <t>connectivity density within a buffer of 300 m</t>
   </si>
   <si>
-    <t>bus_lines_100_y</t>
-  </si>
-  <si>
     <t>length of public bus lines within a buffer of 100 m</t>
   </si>
   <si>
-    <t>bus_lines_300_y</t>
-  </si>
-  <si>
     <t>length of public bus lines within a buffer of 300 m</t>
   </si>
   <si>
-    <t>bus_lines_500_y</t>
-  </si>
-  <si>
     <t>length of public bus lines within a buffer of 500 m</t>
   </si>
   <si>
-    <t>bus_stops_100_y</t>
-  </si>
-  <si>
     <t>number of public bus stops within a buffer of 100 m</t>
   </si>
   <si>
-    <t>bus_stops_300_y</t>
-  </si>
-  <si>
-    <t>number of public bus stops within a buffer of 300 m</t>
-  </si>
-  <si>
-    <t>bus_stops_500_y</t>
-  </si>
-  <si>
     <t>number of public bus stops within a buffer of 500 m</t>
   </si>
   <si>
-    <t>fdensity300_y</t>
-  </si>
-  <si>
     <t>number of facilities present within a buffer of 300 m</t>
   </si>
   <si>
-    <t>frichness300_y</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>number of different facility types present divided by the maximum potential number of facility types within a buffer of 300 m</t>
   </si>
   <si>
-    <t>landuseshan300_y</t>
-  </si>
-  <si>
     <t>landuse Shannon's Evenness Index within a buffer of 300 m</t>
   </si>
   <si>
-    <t>walkability_mean_y</t>
-  </si>
-  <si>
     <t>walkability index (as mean of deciles of facility richness index, landuse shannon's Evenness Index, population density, connectivity density) within a buffer of 300 m</t>
   </si>
   <si>
-    <t>agrgr_y</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>percentage of agrgr (agricultural areas, semi-natural areas and wetlands) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>airpt_y</t>
-  </si>
-  <si>
     <t>percentage of airpt (airports) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>hdres_y</t>
-  </si>
-  <si>
     <t>percentage of hdres (continuous urban fabric) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>indtr_y</t>
-  </si>
-  <si>
     <t>percentage of indtr (industrial, commercial, public, military and private units) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>ldres_y</t>
-  </si>
-  <si>
     <t>percentage of ldres (discontinuous dense/medium density/low density urban fabric) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>natgr_y</t>
-  </si>
-  <si>
     <t>percentage of natgr (forests) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>other_y</t>
-  </si>
-  <si>
     <t>percentage of other (mineral extraction and dump sites, construction sites, land without current use) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>port_y</t>
-  </si>
-  <si>
     <t>percentage of port (port areas) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>trans_y</t>
-  </si>
-  <si>
     <t>percentage of trans (road and rail network and associated land, fast transit roads and associated land, other roads and associated land, railways and associated land) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>urbgr_y</t>
-  </si>
-  <si>
     <t>percentage of urbgr (green urban areas, sports and leisure facilities) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>vldres_y</t>
-  </si>
-  <si>
     <t>percentage of vldres (discontinuous very low density urban fabric) land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>water_y</t>
-  </si>
-  <si>
     <t>percentage of water land use within a buffer of 300 m</t>
   </si>
   <si>
-    <t>blue_dist_y</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
     <t xml:space="preserve"> straight line distance to nearest blue space &gt; 5,000 m2</t>
   </si>
   <si>
-    <t>green_dist_y</t>
-  </si>
-  <si>
     <t xml:space="preserve"> straight line distance to nearest green space &gt; 5,000 m2</t>
   </si>
   <si>
-    <t>blue_size_y</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> area of closest blue space &gt; 5,000m2</t>
   </si>
   <si>
-    <t>green_size_y</t>
-  </si>
-  <si>
     <t xml:space="preserve"> area of closest green space &gt; 5,000m2</t>
   </si>
   <si>
-    <t>blueyn300_y</t>
-  </si>
-  <si>
     <t xml:space="preserve"> is there a blue space  &gt; 5,000 m2 in a distance of 300 m?</t>
   </si>
   <si>
-    <t>greenyn300_y</t>
-  </si>
-  <si>
     <t xml:space="preserve"> is there a green space  &gt; 5,000 m2 in a distance of 300 m?</t>
   </si>
   <si>
-    <t>ndvi100_y</t>
-  </si>
-  <si>
-    <t>ndvi value</t>
-  </si>
-  <si>
     <t>average of NDVI values within a buffer of 100 m</t>
   </si>
   <si>
-    <t>ndvi300_y</t>
-  </si>
-  <si>
     <t>average of NDVI values within a buffer of 300 m</t>
   </si>
   <si>
-    <t>ndvi500_y</t>
-  </si>
-  <si>
     <t>average of NDVI values within a buffer of 500 m</t>
   </si>
   <si>
-    <t>lden_y</t>
-  </si>
-  <si>
-    <t>dB(A)</t>
-  </si>
-  <si>
     <t>day-evening-night level</t>
   </si>
   <si>
-    <t>ln_y</t>
-  </si>
-  <si>
     <t>night level</t>
   </si>
   <si>
-    <t>lden_c_y</t>
-  </si>
-  <si>
     <t>categorized day-evening-night level</t>
   </si>
   <si>
-    <t>ln_c_y</t>
-  </si>
-  <si>
     <t>categorized night level</t>
   </si>
   <si>
-    <t>noise_dist_y</t>
-  </si>
-  <si>
     <t>straight distance to the nearest road with noise level</t>
   </si>
   <si>
-    <t>areases_tert_y</t>
-  </si>
-  <si>
     <t>area-level SES indicator (deprivation index in tertiles)</t>
   </si>
   <si>
-    <t>areases_quint_y</t>
-  </si>
-  <si>
     <t>area-level SES indicator (deprivation index in quintiles)</t>
   </si>
   <si>
-    <t>distinvnear6_y</t>
-  </si>
-  <si>
-    <t>m-1</t>
-  </si>
-  <si>
     <t>inverse distance to nearest road</t>
   </si>
   <si>
-    <t>trafload100_y</t>
-  </si>
-  <si>
-    <t>veh / day m</t>
-  </si>
-  <si>
     <t>total traffic load of all roads within a buffer of 100 m</t>
   </si>
   <si>
-    <t>trafmajorload100_y</t>
-  </si>
-  <si>
     <t>total traffic load of major roads within a buffer of 100 m</t>
   </si>
   <si>
-    <t>trafnear_y</t>
-  </si>
-  <si>
-    <t>veh / day</t>
-  </si>
-  <si>
     <t>traffic density on nearest road</t>
   </si>
   <si>
-    <t>foodenvdens300_y</t>
-  </si>
-  <si>
     <t>number of facilities related to unhealthy food divided by the area of the 300 meters buffer</t>
   </si>
   <si>
-    <t>foodenvdensosm300_y</t>
-  </si>
-  <si>
     <t>number of open street maps facilities related to unhealthy food divided by the area of the 300 meters buffer</t>
   </si>
   <si>
-    <t>tm_y</t>
-  </si>
-  <si>
-    <t>ºC</t>
-  </si>
-  <si>
-    <t>mean temperature</t>
-  </si>
-  <si>
-    <t>tmin_y</t>
-  </si>
-  <si>
-    <t>minimum temperature</t>
-  </si>
-  <si>
-    <t>tmax_y</t>
-  </si>
-  <si>
-    <t>maximum temperature</t>
-  </si>
-  <si>
-    <t>hum_y</t>
-  </si>
-  <si>
-    <t>mean relative humidity</t>
-  </si>
-  <si>
-    <t>hmin_y</t>
-  </si>
-  <si>
-    <t>minimum relative humidity</t>
-  </si>
-  <si>
-    <t>hmax_y</t>
-  </si>
-  <si>
-    <t>maximum relative humidity</t>
-  </si>
-  <si>
-    <t>uvddc_y</t>
-  </si>
-  <si>
-    <t>kJ / sq m</t>
-  </si>
-  <si>
-    <t>DNA-damage UV dose</t>
-  </si>
-  <si>
-    <t>uvdec_y</t>
-  </si>
-  <si>
-    <t>erythemal UV dose</t>
-  </si>
-  <si>
-    <t>uvdvc_y</t>
-  </si>
-  <si>
-    <t>vitamin-d UV dose</t>
-  </si>
-  <si>
-    <t>lst_y</t>
-  </si>
-  <si>
     <t>land surface temperature</t>
   </si>
   <si>
-    <t>FALSO</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -897,6 +558,345 @@
   </si>
   <si>
     <t>medium-high deprivated</t>
+  </si>
+  <si>
+    <t>blueyn300_</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>greenyn300_</t>
+  </si>
+  <si>
+    <t>ln_c_</t>
+  </si>
+  <si>
+    <t>lden_c_</t>
+  </si>
+  <si>
+    <t>areases_tert_</t>
+  </si>
+  <si>
+    <t>areases_quint_</t>
+  </si>
+  <si>
+    <t>no2_</t>
+  </si>
+  <si>
+    <t>micrograms_per_cubic_meter</t>
+  </si>
+  <si>
+    <t>no2 average value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>nox_</t>
+  </si>
+  <si>
+    <t>nox average value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm10_</t>
+  </si>
+  <si>
+    <t>pm10 average value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25_</t>
+  </si>
+  <si>
+    <t>pm25 average value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pmcoarse_</t>
+  </si>
+  <si>
+    <t>pmcoarse average value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25abs_</t>
+  </si>
+  <si>
+    <t>ten_power_minus_five_per_inverse_meter</t>
+  </si>
+  <si>
+    <t>pm25abs average value (extrapolated back in time using ratio method)</t>
+  </si>
+  <si>
+    <t>pm25cu_</t>
+  </si>
+  <si>
+    <t>pm25fe_</t>
+  </si>
+  <si>
+    <t>pm25k_</t>
+  </si>
+  <si>
+    <t>pm25ni_</t>
+  </si>
+  <si>
+    <t>pm25s_</t>
+  </si>
+  <si>
+    <t>pm25si_</t>
+  </si>
+  <si>
+    <t>pm25v_</t>
+  </si>
+  <si>
+    <t>pm25zn_</t>
+  </si>
+  <si>
+    <t>pm10cu_</t>
+  </si>
+  <si>
+    <t>pm10fe_</t>
+  </si>
+  <si>
+    <t>pm10k_</t>
+  </si>
+  <si>
+    <t>pm10ni_</t>
+  </si>
+  <si>
+    <t>pm10s_</t>
+  </si>
+  <si>
+    <t>pm10si_</t>
+  </si>
+  <si>
+    <t>pm10v_</t>
+  </si>
+  <si>
+    <t>pm10zn_</t>
+  </si>
+  <si>
+    <t>popdens_</t>
+  </si>
+  <si>
+    <t>people_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>bdens100_</t>
+  </si>
+  <si>
+    <t>square_meter_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>bdens300_</t>
+  </si>
+  <si>
+    <t>connind100_</t>
+  </si>
+  <si>
+    <t>number_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>connind300_</t>
+  </si>
+  <si>
+    <t>bus_lines_100_</t>
+  </si>
+  <si>
+    <t>meter_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>bus_lines_300_</t>
+  </si>
+  <si>
+    <t>bus_lines_500_</t>
+  </si>
+  <si>
+    <t>bus_stops_100_</t>
+  </si>
+  <si>
+    <t>bus_stops_300_</t>
+  </si>
+  <si>
+    <t>bus_stops_500_</t>
+  </si>
+  <si>
+    <t>fdensity300_</t>
+  </si>
+  <si>
+    <t>frichness300_</t>
+  </si>
+  <si>
+    <t>landuseshan300_</t>
+  </si>
+  <si>
+    <t>walkability_mean_</t>
+  </si>
+  <si>
+    <t>agrgr_</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>airpt_</t>
+  </si>
+  <si>
+    <t>hdres_</t>
+  </si>
+  <si>
+    <t>indtr_</t>
+  </si>
+  <si>
+    <t>ldres_</t>
+  </si>
+  <si>
+    <t>natgr_</t>
+  </si>
+  <si>
+    <t>other_</t>
+  </si>
+  <si>
+    <t>port_</t>
+  </si>
+  <si>
+    <t>trans_</t>
+  </si>
+  <si>
+    <t>urbgr_</t>
+  </si>
+  <si>
+    <t>vldres_</t>
+  </si>
+  <si>
+    <t>water_</t>
+  </si>
+  <si>
+    <t>blue_dist_</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>green_dist_</t>
+  </si>
+  <si>
+    <t>blue_size_</t>
+  </si>
+  <si>
+    <t>square_meter</t>
+  </si>
+  <si>
+    <t>green_size_</t>
+  </si>
+  <si>
+    <t>ndvi100_</t>
+  </si>
+  <si>
+    <t>ndvi_value</t>
+  </si>
+  <si>
+    <t>ndvi300_</t>
+  </si>
+  <si>
+    <t>ndvi500_</t>
+  </si>
+  <si>
+    <t>lden_</t>
+  </si>
+  <si>
+    <t>A_weighted_decibel</t>
+  </si>
+  <si>
+    <t>ln_</t>
+  </si>
+  <si>
+    <t>noise_dist_</t>
+  </si>
+  <si>
+    <t>distinvnear1_</t>
+  </si>
+  <si>
+    <t>inverse_meter</t>
+  </si>
+  <si>
+    <t>trafload100_</t>
+  </si>
+  <si>
+    <t>vehicles_per_day_and_meter</t>
+  </si>
+  <si>
+    <t>trafmajorload100_</t>
+  </si>
+  <si>
+    <t>trafnear_</t>
+  </si>
+  <si>
+    <t>vehicles_per_day</t>
+  </si>
+  <si>
+    <t>foodenvdens300_</t>
+  </si>
+  <si>
+    <t>foodenvdensosm300_</t>
+  </si>
+  <si>
+    <t>tm_</t>
+  </si>
+  <si>
+    <t>degree_celsius</t>
+  </si>
+  <si>
+    <t>average of mean temperature</t>
+  </si>
+  <si>
+    <t>tmin_</t>
+  </si>
+  <si>
+    <t>average of minimum temperature</t>
+  </si>
+  <si>
+    <t>tmax_</t>
+  </si>
+  <si>
+    <t>average of maximum temperature</t>
+  </si>
+  <si>
+    <t>hum_</t>
+  </si>
+  <si>
+    <t>average of mean relative humidity</t>
+  </si>
+  <si>
+    <t>hmin_</t>
+  </si>
+  <si>
+    <t>average of minimum relative humidity</t>
+  </si>
+  <si>
+    <t>hmax_</t>
+  </si>
+  <si>
+    <t>average of maximum relative humidity</t>
+  </si>
+  <si>
+    <t>uvddc_</t>
+  </si>
+  <si>
+    <t>kilojoules_per_square_meter</t>
+  </si>
+  <si>
+    <t>average of DNA-damage UV dose</t>
+  </si>
+  <si>
+    <t>uvdec_</t>
+  </si>
+  <si>
+    <t>average of erythemal UV dose</t>
+  </si>
+  <si>
+    <t>uvdvc_</t>
+  </si>
+  <si>
+    <t>average of vitamin-d UV dose</t>
+  </si>
+  <si>
+    <t>lst_</t>
   </si>
 </sst>
 </file>
@@ -967,7 +967,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -979,6 +979,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1378,7 +1384,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1422,7 +1428,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1446,17 +1452,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BG112"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:D112"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="169.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="15" customHeight="1">
@@ -1980,749 +1986,749 @@
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>103</v>
+        <v>191</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>104</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>106</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>108</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>110</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>111</v>
+        <v>199</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>116</v>
+        <v>203</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>118</v>
+        <v>204</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>122</v>
+        <v>206</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>126</v>
+        <v>208</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>132</v>
+        <v>211</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>134</v>
+        <v>212</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>136</v>
+        <v>213</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>144</v>
+        <v>217</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>157</v>
+        <v>225</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>159</v>
+        <v>226</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>163</v>
+        <v>229</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>173</v>
+        <v>234</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>180</v>
+        <v>237</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>183</v>
+        <v>239</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>184</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>185</v>
+        <v>240</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>186</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="A73" s="3" t="s">
-        <v>189</v>
+        <v>242</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1">
       <c r="A74" s="3" t="s">
-        <v>191</v>
+        <v>243</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>193</v>
+        <v>244</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1">
       <c r="A76" s="3" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>198</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1">
       <c r="A78" s="3" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>200</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1">
       <c r="A79" s="3" t="s">
-        <v>201</v>
+        <v>248</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1">
       <c r="A80" s="3" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="3" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>207</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1">
       <c r="A82" s="3" t="s">
-        <v>208</v>
+        <v>252</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>209</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>210</v>
+        <v>253</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>212</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="3" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>214</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1">
       <c r="A85" s="3" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>3</v>
@@ -2731,12 +2737,12 @@
         <v>4</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>216</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>3</v>
@@ -2745,82 +2751,82 @@
         <v>4</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>218</v>
+        <v>148</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="A87" s="3" t="s">
-        <v>219</v>
+        <v>256</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1">
       <c r="A88" s="3" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>223</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>225</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1">
       <c r="A90" s="3" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1">
       <c r="A91" s="3" t="s">
-        <v>229</v>
+        <v>262</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>230</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1">
       <c r="A92" s="3" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>3</v>
@@ -2829,12 +2835,12 @@
         <v>4</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>232</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1">
       <c r="A93" s="3" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>3</v>
@@ -2843,26 +2849,26 @@
         <v>4</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>234</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1">
       <c r="A94" s="3" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>236</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1">
       <c r="A95" s="3" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>3</v>
@@ -2871,12 +2877,12 @@
         <v>4</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>3</v>
@@ -2885,231 +2891,231 @@
         <v>4</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1">
       <c r="A97" s="3" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>243</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1">
       <c r="A98" s="3" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>246</v>
+        <v>160</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1">
       <c r="A99" s="3" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>248</v>
+        <v>161</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1">
       <c r="A100" s="3" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>251</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1">
       <c r="A101" s="3" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>253</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1">
       <c r="A102" s="3" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>255</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1">
       <c r="A103" s="3" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1">
       <c r="A104" s="3" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="A105" s="3" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1">
       <c r="A106" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1">
       <c r="A107" s="3" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1">
       <c r="A108" s="3" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1">
       <c r="A109" s="3" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1">
       <c r="A110" s="3" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1">
       <c r="A111" s="3" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1">
       <c r="A112" s="3" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>277</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3125,16 +3131,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:D107"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" style="1"/>
-    <col min="4" max="4" width="40.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="8.88671875" style="10"/>
+    <col min="4" max="4" width="45.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -3144,7 +3151,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>97</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -3158,8 +3165,8 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="b">
-        <v>0</v>
+      <c r="C2" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>52</v>
@@ -3172,8 +3179,8 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="b">
-        <v>0</v>
+      <c r="C3" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>53</v>
@@ -3186,8 +3193,8 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="b">
-        <v>0</v>
+      <c r="C4" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>54</v>
@@ -3200,8 +3207,8 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="b">
-        <v>0</v>
+      <c r="C5" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>55</v>
@@ -3214,8 +3221,8 @@
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="b">
-        <v>0</v>
+      <c r="C6" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>56</v>
@@ -3228,8 +3235,8 @@
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="b">
-        <v>0</v>
+      <c r="C7" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>57</v>
@@ -3242,8 +3249,8 @@
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="b">
-        <v>0</v>
+      <c r="C8" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>58</v>
@@ -3256,8 +3263,8 @@
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="b">
-        <v>0</v>
+      <c r="C9" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>59</v>
@@ -3270,8 +3277,8 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="b">
-        <v>0</v>
+      <c r="C10" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>60</v>
@@ -3284,8 +3291,8 @@
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="6" t="b">
-        <v>0</v>
+      <c r="C11" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>61</v>
@@ -3298,8 +3305,8 @@
       <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="6" t="b">
-        <v>0</v>
+      <c r="C12" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>62</v>
@@ -3312,8 +3319,8 @@
       <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="6" t="b">
-        <v>0</v>
+      <c r="C13" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>63</v>
@@ -3326,8 +3333,8 @@
       <c r="B14" s="3">
         <v>5</v>
       </c>
-      <c r="C14" s="6" t="b">
-        <v>0</v>
+      <c r="C14" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>64</v>
@@ -3340,8 +3347,8 @@
       <c r="B15" s="3">
         <v>6</v>
       </c>
-      <c r="C15" s="6" t="b">
-        <v>0</v>
+      <c r="C15" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>65</v>
@@ -3354,8 +3361,8 @@
       <c r="B16" s="3">
         <v>7</v>
       </c>
-      <c r="C16" s="6" t="b">
-        <v>0</v>
+      <c r="C16" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>66</v>
@@ -3368,8 +3375,8 @@
       <c r="B17" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="6" t="b">
-        <v>0</v>
+      <c r="C17" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>67</v>
@@ -3382,8 +3389,8 @@
       <c r="B18" s="3">
         <v>9</v>
       </c>
-      <c r="C18" s="6" t="b">
-        <v>0</v>
+      <c r="C18" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>68</v>
@@ -3396,8 +3403,8 @@
       <c r="B19" s="3">
         <v>0</v>
       </c>
-      <c r="C19" s="6" t="b">
-        <v>0</v>
+      <c r="C19" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>69</v>
@@ -3410,8 +3417,8 @@
       <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="6" t="b">
-        <v>0</v>
+      <c r="C20" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>70</v>
@@ -3424,8 +3431,8 @@
       <c r="B21" s="3">
         <v>2</v>
       </c>
-      <c r="C21" s="6" t="b">
-        <v>0</v>
+      <c r="C21" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>71</v>
@@ -3438,8 +3445,8 @@
       <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="6" t="b">
-        <v>0</v>
+      <c r="C22" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>72</v>
@@ -3452,8 +3459,8 @@
       <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23" s="6" t="b">
-        <v>0</v>
+      <c r="C23" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>73</v>
@@ -3466,8 +3473,8 @@
       <c r="B24" s="3">
         <v>2</v>
       </c>
-      <c r="C24" s="6" t="b">
-        <v>0</v>
+      <c r="C24" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>74</v>
@@ -3480,8 +3487,8 @@
       <c r="B25" s="3">
         <v>3</v>
       </c>
-      <c r="C25" s="6" t="b">
-        <v>0</v>
+      <c r="C25" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>75</v>
@@ -3494,8 +3501,8 @@
       <c r="B26" s="3">
         <v>4</v>
       </c>
-      <c r="C26" s="6" t="b">
-        <v>0</v>
+      <c r="C26" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>76</v>
@@ -3508,8 +3515,8 @@
       <c r="B27" s="3">
         <v>5</v>
       </c>
-      <c r="C27" s="6" t="b">
-        <v>0</v>
+      <c r="C27" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>77</v>
@@ -3522,8 +3529,8 @@
       <c r="B28" s="3">
         <v>6</v>
       </c>
-      <c r="C28" s="6" t="b">
-        <v>0</v>
+      <c r="C28" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>78</v>
@@ -3536,8 +3543,8 @@
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="6" t="b">
-        <v>0</v>
+      <c r="C29" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>6</v>
@@ -3550,8 +3557,8 @@
       <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="6" t="b">
-        <v>0</v>
+      <c r="C30" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>7</v>
@@ -3564,8 +3571,8 @@
       <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="6" t="b">
-        <v>0</v>
+      <c r="C31" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>8</v>
@@ -3578,8 +3585,8 @@
       <c r="B32" s="3">
         <v>4</v>
       </c>
-      <c r="C32" s="6" t="b">
-        <v>0</v>
+      <c r="C32" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>9</v>
@@ -3592,8 +3599,8 @@
       <c r="B33" s="3">
         <v>1</v>
       </c>
-      <c r="C33" s="6" t="b">
-        <v>0</v>
+      <c r="C33" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>73</v>
@@ -3606,8 +3613,8 @@
       <c r="B34" s="3">
         <v>2</v>
       </c>
-      <c r="C34" s="6" t="b">
-        <v>0</v>
+      <c r="C34" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>74</v>
@@ -3620,8 +3627,8 @@
       <c r="B35" s="3">
         <v>3</v>
       </c>
-      <c r="C35" s="6" t="b">
-        <v>0</v>
+      <c r="C35" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>75</v>
@@ -3634,8 +3641,8 @@
       <c r="B36" s="3">
         <v>4</v>
       </c>
-      <c r="C36" s="6" t="b">
-        <v>0</v>
+      <c r="C36" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>76</v>
@@ -3648,8 +3655,8 @@
       <c r="B37" s="3">
         <v>5</v>
       </c>
-      <c r="C37" s="6" t="b">
-        <v>0</v>
+      <c r="C37" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>77</v>
@@ -3662,8 +3669,8 @@
       <c r="B38" s="3">
         <v>6</v>
       </c>
-      <c r="C38" s="6" t="b">
-        <v>0</v>
+      <c r="C38" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>78</v>
@@ -3676,8 +3683,8 @@
       <c r="B39" s="3">
         <v>1</v>
       </c>
-      <c r="C39" s="6" t="b">
-        <v>0</v>
+      <c r="C39" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>6</v>
@@ -3690,8 +3697,8 @@
       <c r="B40" s="3">
         <v>2</v>
       </c>
-      <c r="C40" s="6" t="b">
-        <v>0</v>
+      <c r="C40" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>7</v>
@@ -3704,8 +3711,8 @@
       <c r="B41" s="3">
         <v>3</v>
       </c>
-      <c r="C41" s="6" t="b">
-        <v>0</v>
+      <c r="C41" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>8</v>
@@ -3718,8 +3725,8 @@
       <c r="B42" s="3">
         <v>4</v>
       </c>
-      <c r="C42" s="6" t="b">
-        <v>0</v>
+      <c r="C42" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>9</v>
@@ -3732,8 +3739,8 @@
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="6" t="b">
-        <v>0</v>
+      <c r="C43" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>60</v>
@@ -3746,8 +3753,8 @@
       <c r="B44" s="3">
         <v>2</v>
       </c>
-      <c r="C44" s="6" t="b">
-        <v>0</v>
+      <c r="C44" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>61</v>
@@ -3760,8 +3767,8 @@
       <c r="B45" s="3">
         <v>3</v>
       </c>
-      <c r="C45" s="6" t="b">
-        <v>0</v>
+      <c r="C45" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>62</v>
@@ -3774,8 +3781,8 @@
       <c r="B46" s="3">
         <v>4</v>
       </c>
-      <c r="C46" s="6" t="b">
-        <v>0</v>
+      <c r="C46" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>63</v>
@@ -3788,8 +3795,8 @@
       <c r="B47" s="3">
         <v>5</v>
       </c>
-      <c r="C47" s="6" t="b">
-        <v>0</v>
+      <c r="C47" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>64</v>
@@ -3802,8 +3809,8 @@
       <c r="B48" s="3">
         <v>6</v>
       </c>
-      <c r="C48" s="6" t="b">
-        <v>0</v>
+      <c r="C48" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>65</v>
@@ -3816,8 +3823,8 @@
       <c r="B49" s="3">
         <v>7</v>
       </c>
-      <c r="C49" s="6" t="b">
-        <v>0</v>
+      <c r="C49" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>66</v>
@@ -3830,8 +3837,8 @@
       <c r="B50" s="3">
         <v>8</v>
       </c>
-      <c r="C50" s="6" t="b">
-        <v>0</v>
+      <c r="C50" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>67</v>
@@ -3844,8 +3851,8 @@
       <c r="B51" s="3">
         <v>9</v>
       </c>
-      <c r="C51" s="6" t="b">
-        <v>0</v>
+      <c r="C51" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>68</v>
@@ -3858,8 +3865,8 @@
       <c r="B52" s="3">
         <v>0</v>
       </c>
-      <c r="C52" s="6" t="b">
-        <v>0</v>
+      <c r="C52" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>69</v>
@@ -3872,8 +3879,8 @@
       <c r="B53" s="3">
         <v>1</v>
       </c>
-      <c r="C53" s="6" t="b">
-        <v>0</v>
+      <c r="C53" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>6</v>
@@ -3886,8 +3893,8 @@
       <c r="B54" s="3">
         <v>2</v>
       </c>
-      <c r="C54" s="6" t="b">
-        <v>0</v>
+      <c r="C54" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>7</v>
@@ -3900,8 +3907,8 @@
       <c r="B55" s="3">
         <v>3</v>
       </c>
-      <c r="C55" s="6" t="b">
-        <v>0</v>
+      <c r="C55" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>8</v>
@@ -3914,8 +3921,8 @@
       <c r="B56" s="3">
         <v>4</v>
       </c>
-      <c r="C56" s="6" t="b">
-        <v>0</v>
+      <c r="C56" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>9</v>
@@ -3928,8 +3935,8 @@
       <c r="B57" s="3">
         <v>1</v>
       </c>
-      <c r="C57" s="6" t="b">
-        <v>0</v>
+      <c r="C57" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>60</v>
@@ -3942,8 +3949,8 @@
       <c r="B58" s="3">
         <v>2</v>
       </c>
-      <c r="C58" s="6" t="b">
-        <v>0</v>
+      <c r="C58" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>61</v>
@@ -3956,8 +3963,8 @@
       <c r="B59" s="3">
         <v>3</v>
       </c>
-      <c r="C59" s="6" t="b">
-        <v>0</v>
+      <c r="C59" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>62</v>
@@ -3970,8 +3977,8 @@
       <c r="B60" s="3">
         <v>4</v>
       </c>
-      <c r="C60" s="6" t="b">
-        <v>0</v>
+      <c r="C60" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>63</v>
@@ -3984,8 +3991,8 @@
       <c r="B61" s="3">
         <v>5</v>
       </c>
-      <c r="C61" s="6" t="b">
-        <v>0</v>
+      <c r="C61" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>64</v>
@@ -3998,8 +4005,8 @@
       <c r="B62" s="3">
         <v>6</v>
       </c>
-      <c r="C62" s="6" t="b">
-        <v>0</v>
+      <c r="C62" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>65</v>
@@ -4012,8 +4019,8 @@
       <c r="B63" s="3">
         <v>7</v>
       </c>
-      <c r="C63" s="6" t="b">
-        <v>0</v>
+      <c r="C63" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>66</v>
@@ -4026,8 +4033,8 @@
       <c r="B64" s="3">
         <v>8</v>
       </c>
-      <c r="C64" s="6" t="b">
-        <v>0</v>
+      <c r="C64" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>67</v>
@@ -4040,8 +4047,8 @@
       <c r="B65" s="3">
         <v>9</v>
       </c>
-      <c r="C65" s="6" t="b">
-        <v>0</v>
+      <c r="C65" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>68</v>
@@ -4054,8 +4061,8 @@
       <c r="B66" s="3">
         <v>0</v>
       </c>
-      <c r="C66" s="6" t="b">
-        <v>0</v>
+      <c r="C66" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>69</v>
@@ -4068,8 +4075,8 @@
       <c r="B67" s="3">
         <v>1</v>
       </c>
-      <c r="C67" s="6" t="b">
-        <v>0</v>
+      <c r="C67" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>6</v>
@@ -4082,8 +4089,8 @@
       <c r="B68" s="3">
         <v>2</v>
       </c>
-      <c r="C68" s="6" t="b">
-        <v>0</v>
+      <c r="C68" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>7</v>
@@ -4096,8 +4103,8 @@
       <c r="B69" s="3">
         <v>3</v>
       </c>
-      <c r="C69" s="6" t="b">
-        <v>0</v>
+      <c r="C69" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>8</v>
@@ -4110,8 +4117,8 @@
       <c r="B70" s="3">
         <v>4</v>
       </c>
-      <c r="C70" s="6" t="b">
-        <v>0</v>
+      <c r="C70" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>9</v>
@@ -4124,8 +4131,8 @@
       <c r="B71" s="3">
         <v>1</v>
       </c>
-      <c r="C71" s="6" t="b">
-        <v>0</v>
+      <c r="C71" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>70</v>
@@ -4138,8 +4145,8 @@
       <c r="B72" s="3">
         <v>2</v>
       </c>
-      <c r="C72" s="6" t="b">
-        <v>0</v>
+      <c r="C72" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>71</v>
@@ -4152,8 +4159,8 @@
       <c r="B73" s="3">
         <v>3</v>
       </c>
-      <c r="C73" s="6" t="b">
-        <v>0</v>
+      <c r="C73" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>72</v>
@@ -4166,8 +4173,8 @@
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="6" t="b">
-        <v>0</v>
+      <c r="C74" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>6</v>
@@ -4180,8 +4187,8 @@
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="6" t="b">
-        <v>0</v>
+      <c r="C75" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>7</v>
@@ -4194,8 +4201,8 @@
       <c r="B76" s="3">
         <v>3</v>
       </c>
-      <c r="C76" s="6" t="b">
-        <v>0</v>
+      <c r="C76" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>8</v>
@@ -4208,8 +4215,8 @@
       <c r="B77" s="3">
         <v>4</v>
       </c>
-      <c r="C77" s="6" t="b">
-        <v>0</v>
+      <c r="C77" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>9</v>
@@ -4222,8 +4229,8 @@
       <c r="B78" s="3">
         <v>1</v>
       </c>
-      <c r="C78" s="6" t="b">
-        <v>0</v>
+      <c r="C78" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>70</v>
@@ -4236,8 +4243,8 @@
       <c r="B79" s="3">
         <v>2</v>
       </c>
-      <c r="C79" s="6" t="b">
-        <v>0</v>
+      <c r="C79" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>71</v>
@@ -4250,8 +4257,8 @@
       <c r="B80" s="3">
         <v>3</v>
       </c>
-      <c r="C80" s="6" t="b">
-        <v>0</v>
+      <c r="C80" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>72</v>
@@ -4264,8 +4271,8 @@
       <c r="B81" s="3">
         <v>1</v>
       </c>
-      <c r="C81" s="6" t="b">
-        <v>0</v>
+      <c r="C81" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>6</v>
@@ -4278,8 +4285,8 @@
       <c r="B82" s="3">
         <v>2</v>
       </c>
-      <c r="C82" s="6" t="b">
-        <v>0</v>
+      <c r="C82" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>7</v>
@@ -4292,8 +4299,8 @@
       <c r="B83" s="3">
         <v>3</v>
       </c>
-      <c r="C83" s="6" t="b">
-        <v>0</v>
+      <c r="C83" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>8</v>
@@ -4306,8 +4313,8 @@
       <c r="B84" s="3">
         <v>4</v>
       </c>
-      <c r="C84" s="6" t="b">
-        <v>0</v>
+      <c r="C84" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>9</v>
@@ -4315,324 +4322,324 @@
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1">
       <c r="A85" s="5" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="B85" s="3">
         <v>1</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>279</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1">
       <c r="A86" s="5" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="B86" s="3">
         <v>0</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>280</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="A87" s="5" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B87" s="3">
         <v>1</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>279</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1">
       <c r="A88" s="5" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B88" s="3">
         <v>0</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>280</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1">
       <c r="A89" s="5" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="B89" s="3">
         <v>1</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>281</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1">
       <c r="A90" s="5" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="B90" s="3">
         <v>2</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>282</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1">
       <c r="A91" s="5" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="B91" s="3">
         <v>3</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>283</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1">
       <c r="A92" s="5" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="B92" s="3">
         <v>4</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>284</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1">
       <c r="A93" s="5" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="B93" s="3">
         <v>5</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>285</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1">
       <c r="A94" s="5" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B94" s="3">
         <v>1</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>286</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1">
       <c r="A95" s="5" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B95" s="3">
         <v>2</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>283</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1">
       <c r="A96" s="5" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B96" s="3">
         <v>3</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>284</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1">
       <c r="A97" s="5" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B97" s="3">
         <v>4</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>285</v>
+        <v>172</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1">
       <c r="A98" s="5" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B98" s="3">
         <v>5</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>287</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1">
       <c r="A99" s="5" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="B99" s="3">
         <v>6</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>288</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1">
       <c r="A100" s="5" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B100" s="3">
         <v>1</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>289</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1">
       <c r="A101" s="5" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B101" s="3">
         <v>2</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>290</v>
+        <v>177</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1">
       <c r="A102" s="5" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B102" s="3">
         <v>3</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1">
       <c r="A103" s="5" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B103" s="3">
         <v>1</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>289</v>
+        <v>176</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1">
       <c r="A104" s="5" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B104" s="3">
         <v>2</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>292</v>
+        <v>179</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="A105" s="5" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B105" s="3">
         <v>3</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>290</v>
+        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1">
       <c r="A106" s="5" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B106" s="3">
         <v>4</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>293</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1">
       <c r="A107" s="5" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B107" s="3">
         <v>5</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change text value boolean to boolean value
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ProjectGroups\LifeCycle\Data dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA42449-6C95-AF47-B856-C60BBBAB8BC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="322">
   <si>
     <t>name</t>
   </si>
@@ -506,9 +507,6 @@
   </si>
   <si>
     <t>blueyn300_</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
   <si>
     <t>greenyn300_</t>
@@ -994,7 +992,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1082,8 +1080,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1541,23 +1539,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="169.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="169.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +1624,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1641,12 +1639,12 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4" t="s">
@@ -1654,7 +1652,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1669,7 +1667,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1680,11 +1678,11 @@
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1695,11 +1693,11 @@
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1710,11 +1708,11 @@
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1725,11 +1723,11 @@
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1740,11 +1738,11 @@
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1755,11 +1753,11 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1770,11 +1768,11 @@
         <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1785,11 +1783,11 @@
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1800,11 +1798,11 @@
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1815,11 +1813,11 @@
         <v>4</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1830,11 +1828,11 @@
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -1845,11 +1843,11 @@
         <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1860,11 +1858,11 @@
         <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -1875,11 +1873,11 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>27</v>
       </c>
@@ -1890,11 +1888,11 @@
         <v>4</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -1905,11 +1903,11 @@
         <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1924,7 +1922,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1939,7 +1937,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1954,7 +1952,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1969,7 +1967,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
@@ -1984,7 +1982,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1995,71 +1993,71 @@
         <v>4</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="B28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E27"/>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="E28"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="E29"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>322</v>
-      </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -2070,11 +2068,11 @@
         <v>4</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
@@ -2085,11 +2083,11 @@
         <v>4</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2100,11 +2098,11 @@
         <v>4</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
@@ -2119,7 +2117,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
@@ -2134,485 +2132,485 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37" s="5" t="s">
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" s="5" t="s">
+    </row>
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="B39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" s="5" t="s">
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="B40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D40" s="5" t="s">
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="5" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="B42" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>79</v>
@@ -2624,9 +2622,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>79</v>
@@ -2638,9 +2636,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>3</v>
@@ -2652,231 +2650,231 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>218</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>231</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>161</v>
       </c>
@@ -2890,9 +2888,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>3</v>
@@ -2904,79 +2902,79 @@
         <v>128</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>237</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>3</v>
@@ -2988,9 +2986,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>3</v>
@@ -3002,23 +3000,23 @@
         <v>135</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>3</v>
@@ -3030,9 +3028,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>3</v>
@@ -3044,225 +3042,225 @@
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C102" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C107" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C107" s="4" t="s">
+      <c r="D107" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="D107" s="5" t="s">
+    </row>
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="B108" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D108" s="5" t="s">
+    </row>
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+      <c r="B109" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D109" s="5" t="s">
+    </row>
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+      <c r="B110" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D110" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D110" s="5" t="s">
+    </row>
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="B111" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D111" s="5" t="s">
+    </row>
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="B112" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D112" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B112" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D112" s="5" t="s">
+    </row>
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="B113" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C113" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B113" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C113" s="4" t="s">
+      <c r="D113" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="D113" s="5" t="s">
+    </row>
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="B114" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="B114" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="D114" s="5" t="s">
+    </row>
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+      <c r="B115" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D115" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="B115" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="D115" s="5" t="s">
+    </row>
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="B116" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>145</v>
@@ -3278,23 +3276,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="W68" sqref="W68"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="8.85546875" style="10"/>
-    <col min="4" max="4" width="45.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="8.83203125" style="10"/>
+    <col min="4" max="4" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3308,1821 +3306,1821 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>162</v>
+      <c r="C2" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>162</v>
+      <c r="C3" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>162</v>
+      <c r="C4" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>162</v>
+      <c r="C5" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>162</v>
+      <c r="C6" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>162</v>
+      <c r="C7" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>162</v>
+      <c r="C8" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>162</v>
+      <c r="C9" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>162</v>
+      <c r="C10" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>162</v>
+      <c r="C11" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>162</v>
+      <c r="C12" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>162</v>
+      <c r="C13" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>162</v>
+      <c r="C14" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>6</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>162</v>
+      <c r="C15" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>162</v>
+      <c r="C16" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>162</v>
+      <c r="C17" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>9</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>162</v>
+      <c r="C18" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>162</v>
+      <c r="C19" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>162</v>
+      <c r="C20" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>162</v>
+      <c r="C21" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>162</v>
+      <c r="C22" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>162</v>
+      <c r="C23" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>162</v>
+      <c r="C24" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="3">
         <v>3</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>162</v>
+      <c r="C25" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="3">
         <v>4</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>162</v>
+      <c r="C26" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3">
         <v>5</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>162</v>
+      <c r="C27" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="3">
         <v>6</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>162</v>
+      <c r="C28" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>162</v>
+      <c r="C29" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>162</v>
+      <c r="C30" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>162</v>
+      <c r="C31" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="3">
         <v>4</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>162</v>
+      <c r="C32" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>162</v>
+      <c r="C33" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>162</v>
+      <c r="C34" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="3">
         <v>3</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>162</v>
+      <c r="C35" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="3">
         <v>4</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>162</v>
+      <c r="C36" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="3">
         <v>5</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>162</v>
+      <c r="C37" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="3">
         <v>6</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>162</v>
+      <c r="C38" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>162</v>
+      <c r="C39" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B40" s="3">
         <v>2</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>162</v>
+      <c r="C40" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>162</v>
+      <c r="C41" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B42" s="3">
         <v>4</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>162</v>
+      <c r="C42" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>162</v>
+      <c r="C43" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="3">
         <v>2</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>162</v>
+      <c r="C44" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B45" s="3">
         <v>3</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>162</v>
+      <c r="C45" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="3">
         <v>4</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>162</v>
+      <c r="C46" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="3">
         <v>5</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>162</v>
+      <c r="C47" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B48" s="3">
         <v>6</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>162</v>
+      <c r="C48" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B49" s="3">
         <v>7</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>162</v>
+      <c r="C49" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B50" s="3">
         <v>8</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>162</v>
+      <c r="C50" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B51" s="3">
         <v>9</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>162</v>
+      <c r="C51" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B52" s="3">
         <v>0</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>162</v>
+      <c r="C52" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>162</v>
+      <c r="C53" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="3">
         <v>2</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>162</v>
+      <c r="C54" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B55" s="3">
         <v>3</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>162</v>
+      <c r="C55" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B56" s="3">
         <v>4</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>162</v>
+      <c r="C56" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>162</v>
+      <c r="C57" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B58" s="3">
         <v>2</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>162</v>
+      <c r="C58" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B59" s="3">
         <v>3</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>162</v>
+      <c r="C59" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B60" s="3">
         <v>4</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>162</v>
+      <c r="C60" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B61" s="3">
         <v>5</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>162</v>
+      <c r="C61" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B62" s="3">
         <v>6</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>162</v>
+      <c r="C62" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B63" s="3">
         <v>7</v>
       </c>
-      <c r="C63" s="8" t="s">
-        <v>162</v>
+      <c r="C63" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B64" s="3">
         <v>8</v>
       </c>
-      <c r="C64" s="8" t="s">
-        <v>162</v>
+      <c r="C64" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B65" s="3">
         <v>9</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>162</v>
+      <c r="C65" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B66" s="3">
         <v>0</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>162</v>
+      <c r="C66" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B67" s="3">
         <v>1</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>162</v>
+      <c r="C67" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B68" s="3">
         <v>2</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>162</v>
+      <c r="C68" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B69" s="3">
         <v>3</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>162</v>
+      <c r="C69" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B70" s="3">
         <v>4</v>
       </c>
-      <c r="C70" s="8" t="s">
-        <v>162</v>
+      <c r="C70" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B71" s="3">
         <v>1</v>
       </c>
-      <c r="C71" s="8" t="s">
-        <v>162</v>
+      <c r="C71" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B72" s="3">
         <v>2</v>
       </c>
-      <c r="C72" s="8" t="s">
-        <v>162</v>
+      <c r="C72" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="3">
         <v>3</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>162</v>
+      <c r="C73" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="8" t="s">
-        <v>162</v>
+      <c r="C74" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="8" t="s">
-        <v>162</v>
+      <c r="C75" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B76" s="3">
         <v>3</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>162</v>
+      <c r="C76" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B77" s="3">
         <v>4</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>162</v>
+      <c r="C77" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B78" s="3">
         <v>1</v>
       </c>
-      <c r="C78" s="8" t="s">
-        <v>162</v>
+      <c r="C78" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B79" s="3">
         <v>2</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>162</v>
+      <c r="C79" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B80" s="3">
         <v>3</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>162</v>
+      <c r="C80" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B81" s="3">
         <v>1</v>
       </c>
-      <c r="C81" s="8" t="s">
-        <v>162</v>
+      <c r="C81" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B82" s="3">
         <v>2</v>
       </c>
-      <c r="C82" s="8" t="s">
-        <v>162</v>
+      <c r="C82" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B83" s="3">
         <v>3</v>
       </c>
-      <c r="C83" s="8" t="s">
-        <v>162</v>
+      <c r="C83" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B84" s="3">
         <v>4</v>
       </c>
-      <c r="C84" s="8" t="s">
-        <v>162</v>
+      <c r="C84" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B85" s="3">
         <v>0</v>
       </c>
-      <c r="C85" s="8" t="s">
-        <v>162</v>
+      <c r="C85" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B86" s="3">
         <v>1</v>
       </c>
-      <c r="C86" s="8" t="s">
-        <v>162</v>
+      <c r="C86" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B87" s="3">
         <v>0</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>162</v>
+      <c r="C87" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B88" s="3">
         <v>1</v>
       </c>
-      <c r="C88" s="8" t="s">
-        <v>162</v>
+      <c r="C88" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B89" s="3">
         <v>0</v>
       </c>
-      <c r="C89" s="8" t="s">
-        <v>162</v>
+      <c r="C89" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B90" s="3">
         <v>1</v>
       </c>
-      <c r="C90" s="8" t="s">
-        <v>162</v>
+      <c r="C90" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B91" s="3">
         <v>0</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>162</v>
+      <c r="C91" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B92" s="3">
         <v>1</v>
       </c>
-      <c r="C92" s="8" t="s">
-        <v>162</v>
+      <c r="C92" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B93" s="3">
         <v>0</v>
       </c>
-      <c r="C93" s="8" t="s">
-        <v>162</v>
+      <c r="C93" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B94" s="3">
         <v>1</v>
       </c>
-      <c r="C94" s="8" t="s">
-        <v>162</v>
+      <c r="C94" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B95" s="3">
         <v>0</v>
       </c>
-      <c r="C95" s="8" t="s">
-        <v>162</v>
+      <c r="C95" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B96" s="3">
         <v>1</v>
       </c>
-      <c r="C96" s="8" t="s">
-        <v>162</v>
+      <c r="C96" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B97" s="3">
         <v>0</v>
       </c>
-      <c r="C97" s="8" t="s">
-        <v>162</v>
+      <c r="C97" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B98" s="3">
         <v>1</v>
       </c>
-      <c r="C98" s="8" t="s">
-        <v>162</v>
+      <c r="C98" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B99" s="3">
         <v>0</v>
       </c>
-      <c r="C99" s="8" t="s">
-        <v>162</v>
+      <c r="C99" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B100" s="3">
         <v>1</v>
       </c>
-      <c r="C100" s="8" t="s">
-        <v>162</v>
+      <c r="C100" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B101" s="3">
         <v>0</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>162</v>
+      <c r="C101" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B102" s="3">
         <v>1</v>
       </c>
-      <c r="C102" s="8" t="s">
-        <v>162</v>
+      <c r="C102" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B103" s="3">
         <v>1</v>
       </c>
-      <c r="C103" s="8" t="s">
-        <v>162</v>
+      <c r="C103" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B104" s="3">
         <v>2</v>
       </c>
-      <c r="C104" s="8" t="s">
-        <v>162</v>
+      <c r="C104" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B105" s="3">
         <v>3</v>
       </c>
-      <c r="C105" s="8" t="s">
-        <v>162</v>
+      <c r="C105" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B106" s="3">
         <v>4</v>
       </c>
-      <c r="C106" s="8" t="s">
-        <v>162</v>
+      <c r="C106" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B107" s="3">
         <v>0</v>
       </c>
-      <c r="C107" s="8" t="s">
-        <v>162</v>
+      <c r="C107" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B108" s="3">
         <v>1</v>
       </c>
-      <c r="C108" s="8" t="s">
-        <v>162</v>
+      <c r="C108" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>161</v>
       </c>
       <c r="B109" s="3">
         <v>1</v>
       </c>
-      <c r="C109" s="8" t="s">
-        <v>162</v>
+      <c r="C109" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>161</v>
       </c>
       <c r="B110" s="3">
         <v>0</v>
       </c>
-      <c r="C110" s="8" t="s">
-        <v>162</v>
+      <c r="C110" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B111" s="3">
         <v>1</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>162</v>
+      <c r="C111" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B112" s="3">
         <v>0</v>
       </c>
-      <c r="C112" s="8" t="s">
-        <v>162</v>
+      <c r="C112" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B113" s="3">
         <v>1</v>
       </c>
-      <c r="C113" s="8" t="s">
-        <v>162</v>
+      <c r="C113" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B114" s="3">
         <v>2</v>
       </c>
-      <c r="C114" s="8" t="s">
-        <v>162</v>
+      <c r="C114" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B115" s="3">
         <v>3</v>
       </c>
-      <c r="C115" s="8" t="s">
-        <v>162</v>
+      <c r="C115" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B116" s="3">
         <v>4</v>
       </c>
-      <c r="C116" s="8" t="s">
-        <v>162</v>
+      <c r="C116" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B117" s="3">
         <v>5</v>
       </c>
-      <c r="C117" s="8" t="s">
-        <v>162</v>
+      <c r="C117" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B118" s="3">
         <v>1</v>
       </c>
-      <c r="C118" s="8" t="s">
-        <v>162</v>
+      <c r="C118" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B119" s="3">
         <v>2</v>
       </c>
-      <c r="C119" s="8" t="s">
-        <v>162</v>
+      <c r="C119" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B120" s="3">
         <v>3</v>
       </c>
-      <c r="C120" s="8" t="s">
-        <v>162</v>
+      <c r="C120" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B121" s="3">
         <v>4</v>
       </c>
-      <c r="C121" s="8" t="s">
-        <v>162</v>
+      <c r="C121" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B122" s="3">
         <v>5</v>
       </c>
-      <c r="C122" s="8" t="s">
-        <v>162</v>
+      <c r="C122" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B123" s="3">
         <v>6</v>
       </c>
-      <c r="C123" s="8" t="s">
-        <v>162</v>
+      <c r="C123" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B124" s="3">
         <v>1</v>
       </c>
-      <c r="C124" s="8" t="s">
-        <v>162</v>
+      <c r="C124" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B125" s="3">
         <v>2</v>
       </c>
-      <c r="C125" s="8" t="s">
-        <v>162</v>
+      <c r="C125" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B126" s="3">
         <v>3</v>
       </c>
-      <c r="C126" s="8" t="s">
-        <v>162</v>
+      <c r="C126" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
       </c>
-      <c r="C127" s="8" t="s">
-        <v>162</v>
+      <c r="C127" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B128" s="3">
         <v>2</v>
       </c>
-      <c r="C128" s="8" t="s">
-        <v>162</v>
+      <c r="C128" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B129" s="3">
         <v>3</v>
       </c>
-      <c r="C129" s="8" t="s">
-        <v>162</v>
+      <c r="C129" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B130" s="3">
         <v>4</v>
       </c>
-      <c r="C130" s="8" t="s">
-        <v>162</v>
+      <c r="C130" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B131" s="3">
         <v>5</v>
       </c>
-      <c r="C131" s="8" t="s">
-        <v>162</v>
+      <c r="C131" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
retry for yearly repeated
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_yearly_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA42449-6C95-AF47-B856-C60BBBAB8BC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD78E019-0928-F94C-8BB2-CC8769833954}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3279,7 +3279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A386" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C131"/>
     </sheetView>
   </sheetViews>
@@ -3287,7 +3287,7 @@
   <cols>
     <col min="1" max="1" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="8.83203125" style="10"/>
+    <col min="3" max="3" width="37.5" style="10" customWidth="1"/>
     <col min="4" max="4" width="45.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>

</xml_diff>